<commit_message>
Cambios horarios y excel con NSS
</commit_message>
<xml_diff>
--- a/SistemaVentasBatia/Layouts/ReporteAsistencia.xlsx
+++ b/SistemaVentasBatia/Layouts/ReporteAsistencia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAP_Sistemas5\Desktop\BatiaClientes\SistemaVentasBatia\Layouts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816548A4-B7B6-447E-A16F-988AA9ACE7D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D72A7D-ADAE-435E-A45A-F3A59CC7F1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9F4DFD82-4C49-4107-8358-EC8488FD5DDA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F4DFD82-4C49-4107-8358-EC8488FD5DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Fecha</t>
   </si>
@@ -42,22 +42,28 @@
     <t>Puesto</t>
   </si>
   <si>
-    <t>Hora entrada</t>
-  </si>
-  <si>
-    <t>Hora salida</t>
-  </si>
-  <si>
     <t>Turno</t>
   </si>
   <si>
     <t>Area</t>
+  </si>
+  <si>
+    <t>NSS</t>
+  </si>
+  <si>
+    <t>Entrada</t>
+  </si>
+  <si>
+    <t>Salida</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -87,7 +93,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -101,6 +107,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,52 +428,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B9825A-ADDC-45A5-93E8-24B8837C5768}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7265625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.90625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="36.36328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="27.26953125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="23.6328125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.7265625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="14.36328125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="15.453125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="15.36328125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>6</v>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>